<commit_message>
Updated BoM with resistors and other parts.
</commit_message>
<xml_diff>
--- a/design/schematics/ArmControl/BOM.xlsx
+++ b/design/schematics/ArmControl/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="79">
   <si>
     <t>PART</t>
   </si>
@@ -163,6 +163,96 @@
   </si>
   <si>
     <t>http://www.mouser.com/ProductDetail/Molex/22-43-6030/?qs=%2fha2pyFadujZSIkqFuu9pfAbA%252bc55yEPa0L20yR5s5c%3d</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.7K RESISTOR</t>
+  </si>
+  <si>
+    <t>3.3K RESISTOR</t>
+  </si>
+  <si>
+    <t>7K RESISTOR</t>
+  </si>
+  <si>
+    <t>10K RESISTOR</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay-Thin-Film/PLTT0805Z1721AGT5/?qs=sGAEpiMZZMvdGkrng054t2RPW9MYoEveLabTrIrA%252buo%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Panasonic/ERJ-P6WF3301V/?qs=sGAEpiMZZMvdGkrng054t4TwNrulOmeCGt9o4bxosTAKRbEIXdIPyg%3d%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay/TNPW08057061BT/?qs=sGAEpiMZZMvdGkrng054twN1Uf5gDWJOW9yH6oo%252bIik%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Panasonic/ERJ-P6WF1002V/?qs=sGAEpiMZZMvdGkrng054t4TwNrulOmeC3j4fJE09Xf85wPvNPdhA1w%3d%3d</t>
+  </si>
+  <si>
+    <t>50 RESISTOR</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay/CRCW080550R0FKTA/?qs=aRXG1QX2Yl9J6LSLM7CpJQ%3d%3d</t>
+  </si>
+  <si>
+    <t>370 RESISTOR</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/KOA-Speer/RN73H1ETTP3700F10/?qs=sGAEpiMZZMvdGkrng054t%252bj0%252bMDZxyyPf1KQYUrGN6Q%3d</t>
+  </si>
+  <si>
+    <t>1.5K RESISTOR</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Panasonic/ERJ-2RKF1501X/?qs=sGAEpiMZZMvdGkrng054t8AJgcdMkx7xOyRawAAbetk%3d</t>
+  </si>
+  <si>
+    <t>3.5mm Screw Terminal</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/8084</t>
+  </si>
+  <si>
+    <t>Molex 4 Wire Jumper assembly</t>
+  </si>
+  <si>
+    <t>Encoder connector @ board</t>
+  </si>
+  <si>
+    <t>Encoder connector @ encoder</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/9920</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/9921</t>
+  </si>
+  <si>
+    <t>Molex 5 Wire jumper assembly</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Murata-Electronics/GRM155R61A104KA01D/?qs=sGAEpiMZZMs0AnBnWHyRQEzybnecWqjRhOc0xHRv%252bw8%3d</t>
+  </si>
+  <si>
+    <t>R4,R5,R6,R7,R8,R9,R10,R11,R12,R14</t>
+  </si>
+  <si>
+    <t>R3,R25,R26,R27</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R15,R17,R20,R21,R24</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>R16,R18,R19,R22,R23</t>
   </si>
 </sst>
 </file>
@@ -539,22 +629,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="155.28515625" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
+    <col min="2" max="2" width="24.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="155.33203125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -568,7 +658,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -582,7 +672,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -596,7 +686,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -606,8 +696,11 @@
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
@@ -621,7 +714,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
@@ -635,7 +728,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -649,7 +742,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
@@ -663,7 +756,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
@@ -677,7 +770,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -691,7 +784,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
@@ -705,7 +798,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
@@ -719,7 +812,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>47</v>
       </c>
@@ -733,7 +826,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>43</v>
       </c>
@@ -745,6 +838,113 @@
       </c>
       <c r="D17" s="3" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B28" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B29" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B30" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -772,7 +972,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -784,7 +984,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added BBB, sd card & AX12A servos
</commit_message>
<xml_diff>
--- a/design/schematics/ArmControl/BOM.xlsx
+++ b/design/schematics/ArmControl/BOM.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="88">
   <si>
     <t>PART</t>
   </si>
@@ -151,7 +151,7 @@
     <t>AX-12A</t>
   </si>
   <si>
-    <t>SPOX-3 for AX-12A </t>
+    <t>SPOX-3 for AX-12A</t>
   </si>
   <si>
     <t>http://www.mouser.com/ProductDetail/Molex/22-43-6030/?qs=%2fha2pyFadujZSIkqFuu9pfAbA%252bc55yEPa0L20yR5s5c%3d</t>
@@ -172,7 +172,7 @@
     <t>R15,R17,R20,R21,R24</t>
   </si>
   <si>
-    <t> 1.7K RESISTOR</t>
+    <t>1.7K RESISTOR</t>
   </si>
   <si>
     <t>http://www.mouser.com/ProductDetail/Vishay-Thin-Film/PLTT0805Z1721AGT5/?qs=sGAEpiMZZMvdGkrng054t2RPW9MYoEveLabTrIrA%252buo%3d</t>
@@ -263,6 +263,24 @@
   </si>
   <si>
     <t>http://www.mouser.com/ProductDetail/STMicroelectronics/LD1085D2T-R/?qs=sGAEpiMZZMsGz1a6aV8DcNi9%252bTg6j2AWastsvd5jJkk%3d</t>
+  </si>
+  <si>
+    <t>USD-CARDS</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Apacer/AP16GMCSH4-B/?qs=sGAEpiMZZMtyMAXUUxCBE4AZ7JbBE3hTRlqQ2Hq7Z8o%3d</t>
+  </si>
+  <si>
+    <t>BBB (3)</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/new/embedded-solutions/beagleboneblack/n-5g1kZ2bv0qx</t>
+  </si>
+  <si>
+    <t>AX-12A (1)</t>
+  </si>
+  <si>
+    <t>http://www.trossenrobotics.com/dynamixel-ax-12-robot-actuator.aspx</t>
   </si>
 </sst>
 </file>
@@ -394,7 +412,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Heading 1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Heading 1" xfId="21" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
@@ -465,9 +483,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -785,16 +803,19 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0"/>
       <c r="B26" s="0"/>
       <c r="C26" s="0"/>
       <c r="D26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0"/>
       <c r="B27" s="0"/>
       <c r="C27" s="0"/>
       <c r="D27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0"/>
       <c r="B28" s="1" t="s">
         <v>71</v>
       </c>
@@ -804,6 +825,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0"/>
       <c r="B29" s="1" t="s">
         <v>73</v>
       </c>
@@ -815,6 +837,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0"/>
       <c r="B30" s="1" t="s">
         <v>76</v>
       </c>
@@ -824,6 +847,12 @@
       <c r="D30" s="1" t="s">
         <v>78</v>
       </c>
+    </row>
+    <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0"/>
+      <c r="B31" s="0"/>
+      <c r="C31" s="0"/>
+      <c r="D31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
@@ -837,6 +866,30 @@
       </c>
       <c r="D32" s="1" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed part number for NPN xtors
</commit_message>
<xml_diff>
--- a/design/schematics/ArmControl/BOM.xlsx
+++ b/design/schematics/ArmControl/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -159,9 +159,6 @@
     <t>T1 to T6</t>
   </si>
   <si>
-    <t>BF820-NPN-SOT23-BEC</t>
-  </si>
-  <si>
     <t>NPN Transistors</t>
   </si>
   <si>
@@ -286,6 +283,9 @@
   </si>
   <si>
     <t>http://www.mouser.com/ProductDetail/NXP/BC846215/?qs=%2fha2pyFadujuUAn4sl%2fZ3HIadiACA4SYaUXXifegWq7CBv9Mh%252bf%252blQ%3d%3d</t>
+  </si>
+  <si>
+    <t>BC846-NPN-SOT23-BEC</t>
   </si>
 </sst>
 </file>
@@ -736,21 +736,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:E36"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="30" style="3" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" style="3"/>
+    <col min="3" max="3" width="32.109375" style="3"/>
     <col min="4" max="4" width="26" style="3" customWidth="1"/>
-    <col min="5" max="5" width="139.28515625" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="3"/>
+    <col min="5" max="5" width="139.33203125" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -761,13 +761,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -784,7 +784,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -801,7 +801,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -818,7 +818,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -835,7 +835,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
@@ -852,7 +852,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -863,13 +863,13 @@
         <v>23</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>25</v>
       </c>
@@ -880,13 +880,13 @@
         <v>26</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
@@ -897,13 +897,13 @@
         <v>29</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>31</v>
       </c>
@@ -914,13 +914,13 @@
         <v>32</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>34</v>
       </c>
@@ -937,7 +937,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>38</v>
       </c>
@@ -954,7 +954,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>42</v>
       </c>
@@ -971,211 +971,211 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="D17" s="3">
         <v>25</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="D19" s="3">
         <v>25</v>
       </c>
       <c r="E19" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="D20" s="3">
         <v>25</v>
       </c>
       <c r="E20" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="D21" s="3">
         <v>10</v>
       </c>
       <c r="E21" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="D22" s="3">
         <v>25</v>
       </c>
       <c r="E22" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="D23" s="3">
         <v>25</v>
       </c>
       <c r="E23" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="B24" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="D24" s="3">
         <v>25</v>
       </c>
       <c r="E24" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="D25" s="3">
         <v>25</v>
       </c>
       <c r="E25" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B28" s="3" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="D28" s="3">
         <v>15</v>
       </c>
       <c r="E28" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B29" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="D29" s="3">
         <v>10</v>
       </c>
       <c r="E29" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B30" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="D30" s="3">
         <v>10</v>
       </c>
       <c r="E30" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="B32" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="C32" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D32" s="3">
         <v>5</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E33" s="4"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D34" s="3">
         <v>2</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D35" s="3">
         <v>2</v>
       </c>
       <c r="E35" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="D36" s="3">
         <v>1</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1219,9 +1219,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1025" width="8.5703125"/>
+    <col min="1" max="1025" width="8.5546875"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1235,9 +1235,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1025" width="8.5703125"/>
+    <col min="1" max="1025" width="8.5546875"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
updated BoM with easier to obtain 374 ohm resistor
</commit_message>
<xml_diff>
--- a/design/schematics/ArmControl/BOM.xlsx
+++ b/design/schematics/ArmControl/BOM.xlsx
@@ -213,9 +213,6 @@
     <t>370 RESISTOR</t>
   </si>
   <si>
-    <t>http://www.mouser.com/ProductDetail/KOA-Speer/RN73H1ETTP3700F10/?qs=sGAEpiMZZMvdGkrng054t%252bj0%252bMDZxyyPf1KQYUrGN6Q%3d</t>
-  </si>
-  <si>
     <t>R2</t>
   </si>
   <si>
@@ -286,6 +283,9 @@
   </si>
   <si>
     <t>BC846-NPN-SOT23-BEC</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Panasonic/ERJ-2RKF3740X/?qs=sGAEpiMZZMvdGkrng054t8AJgcdMkx7x12YxA1eMwik%3d</t>
   </si>
 </sst>
 </file>
@@ -736,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="C8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -761,7 +761,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -863,7 +863,7 @@
         <v>23</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>24</v>
@@ -880,7 +880,7 @@
         <v>26</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>27</v>
@@ -897,7 +897,7 @@
         <v>29</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>30</v>
@@ -914,7 +914,7 @@
         <v>32</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>33</v>
@@ -976,7 +976,7 @@
         <v>46</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>47</v>
@@ -985,7 +985,7 @@
         <v>25</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1069,77 +1069,77 @@
         <v>25</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="D25" s="3">
         <v>25</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D28" s="3">
         <v>15</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="D29" s="3">
         <v>10</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="D30" s="3">
         <v>10</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="C32" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D32" s="3">
         <v>5</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1147,35 +1147,35 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D34" s="3">
         <v>2</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D35" s="3">
         <v>2</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D36" s="3">
         <v>1</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1197,16 +1197,15 @@
     <hyperlink ref="E25" r:id="rId15"/>
     <hyperlink ref="E29" r:id="rId16"/>
     <hyperlink ref="E22" r:id="rId17"/>
-    <hyperlink ref="E24" r:id="rId18"/>
-    <hyperlink ref="E28" r:id="rId19"/>
-    <hyperlink ref="E30" r:id="rId20"/>
-    <hyperlink ref="E32" r:id="rId21"/>
-    <hyperlink ref="E34" r:id="rId22"/>
-    <hyperlink ref="E35" r:id="rId23"/>
-    <hyperlink ref="E36" r:id="rId24"/>
-    <hyperlink ref="E17" r:id="rId25"/>
-    <hyperlink ref="E3" r:id="rId26"/>
-    <hyperlink ref="E4" r:id="rId27"/>
+    <hyperlink ref="E28" r:id="rId18"/>
+    <hyperlink ref="E30" r:id="rId19"/>
+    <hyperlink ref="E32" r:id="rId20"/>
+    <hyperlink ref="E34" r:id="rId21"/>
+    <hyperlink ref="E35" r:id="rId22"/>
+    <hyperlink ref="E36" r:id="rId23"/>
+    <hyperlink ref="E17" r:id="rId24"/>
+    <hyperlink ref="E3" r:id="rId25"/>
+    <hyperlink ref="E4" r:id="rId26"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>